<commit_message>
data analysis for odometry data
</commit_message>
<xml_diff>
--- a/data/omni-control/simtwo/gt/data-analysis_gt.xlsx
+++ b/data/omni-control/simtwo/gt/data-analysis_gt.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="724" documentId="8_{6C4C5C12-CB74-4A7B-923B-BE3379E350DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DE03037-578B-4512-8D5F-CF9BE0544B69}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{FD07EEC4-0C01-44C2-8089-ACB43FE9EBFC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FD07EEC4-0C01-44C2-8089-ACB43FE9EBFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1206,7 +1206,7 @@
   <dimension ref="A1:U199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="5" ySplit="13" topLeftCell="F76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="13" topLeftCell="F124" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
       <selection pane="bottomRight" activeCell="A76" sqref="A76:A137"/>

</xml_diff>